<commit_message>
descw-1279 get main query working
* also got frontend queryselector working
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_2_rpt_CA_ActiveContractorList.xlsx
+++ b/backend/reports/xlsx/Tab_2_rpt_CA_ActiveContractorList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF88463-F804-B54F-9BFE-C85CA09996B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3FBAE31-3534-D347-BA93-445F4041841B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="29940" windowHeight="18660" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>{#fy=d.fiscal_year}</t>
   </si>
   <si>
-    <t>Contractor Resource List (Active) as of {$date}</t>
-  </si>
-  <si>
     <t>Contractor Name</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
   </si>
   <si>
     <t>{#c1=d.report[i].contractors[i+1]}</t>
+  </si>
+  <si>
+    <t>Active Contractor Resource List</t>
   </si>
 </sst>
 </file>
@@ -744,7 +744,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C1" sqref="C1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -760,7 +760,7 @@
       <c r="A1" s="8"/>
       <c r="B1" s="8"/>
       <c r="C1" s="9" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -769,28 +769,28 @@
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="33" thickBot="1">
       <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="2" customFormat="1" ht="20" thickBot="1">
       <c r="A3" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -801,30 +801,30 @@
     </row>
     <row r="4" spans="1:7" s="2" customFormat="1" ht="20" thickBot="1">
       <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="D4" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="E4" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="F4" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="G4" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" ht="20" thickBot="1">
       <c r="A5" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="19"/>
@@ -835,7 +835,7 @@
     </row>
     <row r="6" spans="1:7" ht="17" thickBot="1">
       <c r="A6" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -861,12 +861,12 @@
     </row>
     <row r="12" spans="1:7">
       <c r="B12" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="B13" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:7">

</xml_diff>